<commit_message>
done readme, final admin changes
</commit_message>
<xml_diff>
--- a/admin/BoM.xlsx
+++ b/admin/BoM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncanboyd/Documents/Projects/Foghorn/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/duncanboyd/Documents/GitRepos/foghorn/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF0CD48-B860-8745-90E8-89AFB06E0BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742426A5-5AE5-1F49-8DB5-BA05D89E2E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16720" xr2:uid="{16B7AFF6-DB58-C340-9195-EC2C510A6DC4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Item</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>https://www.amazon.ca/ESP32-C6-Microcontroller-1-47inch-Colorful-Applications/dp/B0DHVQYFGM</t>
+  </si>
+  <si>
+    <t>Replacement Screen and Solder</t>
   </si>
 </sst>
 </file>
@@ -186,8 +189,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A4215C8-148E-D846-BDE5-3DA17D72A990}" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:C12" xr:uid="{2A4215C8-148E-D846-BDE5-3DA17D72A990}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2A4215C8-148E-D846-BDE5-3DA17D72A990}" name="Table1" displayName="Table1" ref="A1:C13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:C13" xr:uid="{2A4215C8-148E-D846-BDE5-3DA17D72A990}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{90E0BF62-B8B7-E441-B475-DECDEEF6AA30}" name="Item"/>
     <tableColumn id="3" xr3:uid="{EC69038A-B43C-854C-A72D-A081959A1251}" name="Cost (CAD)"/>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549AD11D-6930-5246-AFB7-E11EE8165B1F}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +546,7 @@
       </c>
       <c r="F1">
         <f>SUM(B:B)</f>
-        <v>106.59020000000001</v>
+        <v>127.03020000000001</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -656,6 +659,17 @@
         <v>0.37</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>20.440000000000001</v>
+      </c>
+      <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>